<commit_message>
Organize macros into kafka v2
</commit_message>
<xml_diff>
--- a/scripts/inputs_qserver_kafka_v2.xlsx
+++ b/scripts/inputs_qserver_kafka_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenghunglin/Documents/Git_BNL/profile_collection_ldrd20-31/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E8E0EE-A8C9-0A45-8890-FA35899764C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F24DF7-A92B-7040-911F-E3C98BC97F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="1440" windowWidth="35140" windowHeight="21720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12120" yWindow="4940" windowWidth="35140" windowHeight="21720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="qserver_XPD" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="163">
   <si>
     <t>Input parameters for tasks in queue server</t>
   </si>
@@ -372,9 +372,6 @@
   </si>
   <si>
     <t>sandbox_tiled_client</t>
-  </si>
-  <si>
-    <t>tiled_client</t>
   </si>
   <si>
     <t>fn_TBD</t>
@@ -555,6 +552,12 @@
   </si>
   <si>
     <t>dummy_pdf</t>
+  </si>
+  <si>
+    <t>beamline_acronym</t>
+  </si>
+  <si>
+    <t>fix_Br_ratio</t>
   </si>
 </sst>
 </file>
@@ -1118,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1576,7 +1579,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2031,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2180,161 +2183,170 @@
       <c r="B15">
         <v>1</v>
       </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
         <v>80</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
         <v>83</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>515</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
+      <c r="C21">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" t="s">
-        <v>86</v>
+        <v>84</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
         <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
         <v>85</v>
       </c>
       <c r="C27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
         <v>96</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
-        <v>98</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
         <v>99</v>
       </c>
       <c r="C36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
-        <v>161</v>
-      </c>
-      <c r="B38">
-        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>160</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -2342,25 +2354,28 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>107</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
         <v>87</v>
@@ -2380,7 +2395,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B40" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B41" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2392,7 +2407,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2549,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -2557,7 +2572,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -2565,23 +2580,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>83</v>
       </c>
       <c r="B20">
         <v>515</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
         <v>112</v>
       </c>
-      <c r="B21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>84</v>
       </c>
@@ -2589,39 +2607,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>93</v>
       </c>
@@ -2629,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>94</v>
       </c>
@@ -2637,7 +2655,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>96</v>
       </c>
@@ -2655,7 +2673,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B34" t="s">
         <v>100</v>
@@ -2663,18 +2681,18 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" t="s">
         <v>119</v>
-      </c>
-      <c r="B35" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" t="s">
         <v>121</v>
-      </c>
-      <c r="B36" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
@@ -2698,7 +2716,7 @@
         <v>109</v>
       </c>
       <c r="B40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2712,7 +2730,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2726,12 +2744,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2991,7 +3009,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B18">
         <v>36</v>
@@ -3448,21 +3466,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
         <v>128</v>
-      </c>
-      <c r="C2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -3470,7 +3488,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -3478,7 +3496,7 @@
         <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
@@ -3486,7 +3504,7 @@
         <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -3494,7 +3512,7 @@
         <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
@@ -3502,7 +3520,7 @@
         <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
@@ -3510,7 +3528,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
@@ -3518,7 +3536,7 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
@@ -3526,7 +3544,7 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
@@ -3534,7 +3552,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
@@ -3542,7 +3560,7 @@
         <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
@@ -3550,7 +3568,7 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
@@ -3558,7 +3576,7 @@
         <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -3566,7 +3584,7 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
@@ -3574,7 +3592,7 @@
         <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
@@ -3582,7 +3600,7 @@
         <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
@@ -3590,7 +3608,7 @@
         <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
@@ -3598,7 +3616,7 @@
         <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
@@ -3606,7 +3624,7 @@
         <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
@@ -3614,7 +3632,7 @@
         <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
@@ -3622,7 +3640,7 @@
         <v>56</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3653,12 +3671,12 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3669,7 +3687,7 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
@@ -3768,13 +3786,13 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" t="s">
         <v>150</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>151</v>
-      </c>
-      <c r="D9" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
@@ -3824,10 +3842,10 @@
         <v>35</v>
       </c>
       <c r="B13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" t="s">
         <v>153</v>
-      </c>
-      <c r="C13" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
@@ -3852,7 +3870,7 @@
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E15">
         <v>300</v>
@@ -3871,13 +3889,13 @@
         <v>55</v>
       </c>
       <c r="B17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" t="s">
         <v>156</v>
-      </c>
-      <c r="C17" t="s">
-        <v>156</v>
-      </c>
-      <c r="D17" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -3885,13 +3903,13 @@
         <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
@@ -3899,13 +3917,13 @@
         <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
@@ -3913,13 +3931,13 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
test work flow at 1LL09 with macros
</commit_message>
<xml_diff>
--- a/scripts/inputs_qserver_kafka_v2.xlsx
+++ b/scripts/inputs_qserver_kafka_v2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="167">
   <si>
     <t xml:space="preserve">Input parameters for tasks in queue server</t>
   </si>
@@ -56,6 +56,9 @@
     <t xml:space="preserve">back</t>
   </si>
   <si>
+    <t xml:space="preserve">use_OAm</t>
+  </si>
+  <si>
     <t xml:space="preserve">name_by_prefix</t>
   </si>
   <si>
@@ -152,61 +155,61 @@
     <t xml:space="preserve">wash_tube</t>
   </si>
   <si>
+    <t xml:space="preserve">200 ul/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 ul/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resident_t_ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate_unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uvvis_config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qepro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perkin_config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">det</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auto_set_target_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set_target_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infuse_rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp://xf28id2-ca2:60615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp://xf28id2-ca2:60625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OAm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dds3_p2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dds3_p1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OAm_Tol</t>
+  </si>
+  <si>
     <t xml:space="preserve">ultra2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200 ul/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 ul/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resident_t_ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rate_unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ul/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uvvis_config</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qepro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">perkin_config</t>
-  </si>
-  <si>
-    <t xml:space="preserve">det</t>
-  </si>
-  <si>
-    <t xml:space="preserve">auto_set_target_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set_target_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infuse_rates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tcp://xf28id2-ca2:60615</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tcp://xf28id2-ca2:60625</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OAm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dds3_p2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dds3_p1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OAm_Tol</t>
   </si>
   <si>
     <t xml:space="preserve">Input parameters for data process in kafka</t>
@@ -866,16 +869,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.66"/>
@@ -930,151 +933,144 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>14</v>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="4" t="n">
-        <v>50</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="E15" s="5" t="n">
-        <v>50</v>
+      <c r="C15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="D17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="E17" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="B19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="9" t="n">
-        <v>30</v>
-      </c>
-      <c r="C20" s="9" t="n">
-        <v>20</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -1084,136 +1080,133 @@
       <c r="A21" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>39</v>
-      </c>
+      <c r="B21" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="C21" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="0" t="n">
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="0" t="s">
+      <c r="D23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F23" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G23" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="0" t="s">
+      <c r="H23" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="0" t="n">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>0.05</v>
+      <c r="I23" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>0.05</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B27" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C27" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D27" s="0" t="n">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C31" s="10" t="n">
-        <v>167</v>
-      </c>
-      <c r="D31" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="E31" s="0" t="n">
-        <f aca="false">SUM(B31:D31)*5</f>
-        <v>1500</v>
-      </c>
-    </row>
+      <c r="B30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>53</v>
@@ -1250,8 +1243,26 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="10" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" s="10" t="n">
+        <v>167</v>
+      </c>
+      <c r="D34" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <f aca="false">SUM(B34:D34)*5</f>
+        <v>1500</v>
+      </c>
+    </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1268,16 +1279,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.66"/>
@@ -1332,169 +1343,162 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>14</v>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="4" t="n">
-        <v>50</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="F15" s="5" t="n">
-        <v>50</v>
+      <c r="C15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="D17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="9" t="s">
+      <c r="F17" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="B19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="9" t="n">
-        <v>30</v>
-      </c>
-      <c r="C20" s="9" t="n">
-        <v>20</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -1504,142 +1508,136 @@
       <c r="A21" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>39</v>
-      </c>
+      <c r="B21" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="C21" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <v>360</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>2</v>
+        <v>50</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>360</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B27" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C27" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D27" s="0" t="n">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C31" s="10" t="n">
-        <v>167</v>
-      </c>
-      <c r="D31" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="E31" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <f aca="false">SUM(B31:E31)*5</f>
-        <v>1500</v>
-      </c>
-    </row>
+      <c r="B30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>53</v>
@@ -1654,11 +1652,11 @@
         <v>100</v>
       </c>
       <c r="E32" s="10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F32" s="0" t="n">
         <f aca="false">SUM(B32:E32)*5</f>
-        <v>1550</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1675,15 +1673,36 @@
         <v>100</v>
       </c>
       <c r="E33" s="10" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="false">SUM(B33:E33)*5</f>
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="10" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" s="10" t="n">
+        <v>167</v>
+      </c>
+      <c r="D34" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="E34" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <f aca="false">SUM(B34:E34)*5</f>
         <v>1600</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1700,13 +1719,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -1763,169 +1782,162 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>14</v>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="4" t="n">
-        <v>50</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="F15" s="5" t="n">
-        <v>50</v>
+      <c r="C15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="D17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="9" t="s">
+      <c r="F17" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="B19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="9" t="n">
-        <v>30</v>
-      </c>
-      <c r="C20" s="9" t="n">
-        <v>20</v>
-      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -1935,143 +1947,137 @@
       <c r="A21" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>39</v>
-      </c>
+      <c r="B21" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="C21" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <v>360</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>2</v>
+        <v>50</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>360</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B27" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C27" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D27" s="0" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
+      <c r="B30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C31" s="10" t="n">
-        <v>167</v>
-      </c>
-      <c r="D31" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="E31" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <f aca="false">SUM(B31:E31)*5</f>
-        <v>1500</v>
-      </c>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -2087,11 +2093,11 @@
         <v>100</v>
       </c>
       <c r="E32" s="10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F32" s="0" t="n">
         <f aca="false">SUM(B32:E32)*5</f>
-        <v>1550</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,15 +2114,36 @@
         <v>100</v>
       </c>
       <c r="E33" s="10" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="false">SUM(B33:E33)*5</f>
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="10" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" s="10" t="n">
+        <v>167</v>
+      </c>
+      <c r="D34" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="E34" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <f aca="false">SUM(B34:E34)*5</f>
         <v>1600</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2135,27 +2162,27 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -2163,15 +2190,15 @@
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>50</v>
@@ -2179,7 +2206,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>40</v>
@@ -2187,7 +2214,7 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>30</v>
@@ -2195,13 +2222,13 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>365</v>
@@ -2221,66 +2248,66 @@
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -2291,7 +2318,7 @@
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -2302,7 +2329,7 @@
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -2310,23 +2337,23 @@
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>585</v>
@@ -2337,7 +2364,7 @@
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -2345,48 +2372,48 @@
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0</v>
@@ -2394,23 +2421,23 @@
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>0</v>
@@ -2418,37 +2445,37 @@
     </row>
     <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -2456,7 +2483,7 @@
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>0</v>
@@ -2464,35 +2491,35 @@
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2520,7 +2547,7 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.48"/>
@@ -2530,12 +2557,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -2543,15 +2570,15 @@
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>50</v>
@@ -2559,7 +2586,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>40</v>
@@ -2567,7 +2594,7 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>30</v>
@@ -2575,13 +2602,13 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>365</v>
@@ -2601,58 +2628,58 @@
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -2660,7 +2687,7 @@
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -2668,7 +2695,7 @@
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -2676,15 +2703,15 @@
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -2692,7 +2719,7 @@
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>515</v>
@@ -2703,15 +2730,15 @@
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -2719,39 +2746,39 @@
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -2759,23 +2786,23 @@
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
@@ -2783,31 +2810,31 @@
     </row>
     <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
@@ -2815,7 +2842,7 @@
     </row>
     <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
@@ -2823,10 +2850,10 @@
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2851,7 +2878,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -2862,12 +2889,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -2878,15 +2905,15 @@
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>50</v>
@@ -2894,7 +2921,7 @@
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>40</v>
@@ -2902,7 +2929,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>30</v>
@@ -2910,13 +2937,13 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>365</v>
@@ -2936,39 +2963,39 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>56</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>57</v>
@@ -2979,47 +3006,47 @@
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>59</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>50</v>
@@ -3039,36 +3066,36 @@
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -3076,18 +3103,18 @@
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -3096,7 +3123,7 @@
         <v>50</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>42</v>
@@ -3105,7 +3132,7 @@
         <v>20</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>43</v>
@@ -3127,7 +3154,7 @@
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>36</v>
@@ -3579,7 +3606,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="78.65"/>
@@ -3588,125 +3615,125 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3714,7 +3741,7 @@
         <v>44</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3722,7 +3749,7 @@
         <v>53</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3730,7 +3757,7 @@
         <v>53</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3738,7 +3765,7 @@
         <v>53</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3746,7 +3773,7 @@
         <v>52</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3754,7 +3781,7 @@
         <v>52</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3762,7 +3789,7 @@
         <v>52</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3787,7 +3814,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>
@@ -3797,12 +3824,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -3810,15 +3837,15 @@
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>150</v>
@@ -3835,7 +3862,7 @@
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>100</v>
@@ -3852,7 +3879,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>70</v>
@@ -3869,13 +3896,13 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>365</v>
@@ -3895,49 +3922,49 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>50</v>
@@ -3951,52 +3978,52 @@
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>50</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>300</v>
@@ -4015,13 +4042,13 @@
         <v>53</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4029,13 +4056,13 @@
         <v>53</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4043,13 +4070,13 @@
         <v>53</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4057,13 +4084,13 @@
         <v>53</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
test pdf fitting at 1LL09 with macros
</commit_message>
<xml_diff>
--- a/scripts/inputs_qserver_kafka_v2.xlsx
+++ b/scripts/inputs_qserver_kafka_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="qserver_test" sheetId="1" state="visible" r:id="rId2"/>
@@ -871,11 +871,11 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1285,7 +1285,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1725,7 +1725,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -2162,11 +2162,11 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
@@ -2486,7 +2486,7 @@
         <v>109</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2547,7 +2547,7 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.48"/>
@@ -2878,7 +2878,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -3606,7 +3606,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="78.65"/>
@@ -3814,7 +3814,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>

</xml_diff>

<commit_message>
test export and save kafka info as log
</commit_message>
<xml_diff>
--- a/scripts/inputs_qserver_kafka_v2.xlsx
+++ b/scripts/inputs_qserver_kafka_v2.xlsx
@@ -875,7 +875,7 @@
       <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1285,7 +1285,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1725,7 +1725,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -2162,11 +2162,11 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
@@ -2486,7 +2486,7 @@
         <v>109</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2547,7 +2547,7 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.48"/>
@@ -2878,7 +2878,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -3606,7 +3606,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="78.65"/>
@@ -3814,7 +3814,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>

</xml_diff>

<commit_message>
debug workflow at beamline for two topics
</commit_message>
<xml_diff>
--- a/scripts/inputs_qserver_kafka_v2.xlsx
+++ b/scripts/inputs_qserver_kafka_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="qserver_test" sheetId="1" state="visible" r:id="rId2"/>
@@ -874,8 +874,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1084,10 +1084,10 @@
         <v>37</v>
       </c>
       <c r="B21" s="9" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C21" s="9" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -2165,8 +2165,8 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2370,7 +2370,7 @@
         <v>88</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2419,7 +2419,7 @@
         <v>97</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,7 +2443,7 @@
         <v>102</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2489,7 +2489,7 @@
         <v>110</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
test macros with 100 mM TOABr
</commit_message>
<xml_diff>
--- a/scripts/inputs_qserver_kafka_v2.xlsx
+++ b/scripts/inputs_qserver_kafka_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="qserver_test" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="174">
   <si>
     <t xml:space="preserve">Input parameters for tasks in queue server</t>
   </si>
@@ -215,6 +215,18 @@
     <t xml:space="preserve">tcp://localhost:60625</t>
   </si>
   <si>
+    <t xml:space="preserve">CsPb(oleate)3_30mM_20240503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOABr_100mM_20240814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZnCl2_60mM_20240701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 ml</t>
+  </si>
+  <si>
     <t xml:space="preserve">Input parameters for data process in kafka</t>
   </si>
   <si>
@@ -224,7 +236,7 @@
     <t xml:space="preserve">csv_path</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/20240812_v2_test</t>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/20240820_macro_Br</t>
   </si>
   <si>
     <t xml:space="preserve">key_height</t>
@@ -266,6 +278,9 @@
     <t xml:space="preserve">infusion_rate_Cl</t>
   </si>
   <si>
+    <t xml:space="preserve">infusion_rate_OAm</t>
+  </si>
+  <si>
     <t xml:space="preserve">new_points_label</t>
   </si>
   <si>
@@ -284,7 +299,10 @@
     <t xml:space="preserve">agent_data_path</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/202405_halide_data/20240520_21_I</t>
+    <t xml:space="preserve">/home/xf28id2/data_post_dilute_100mM_PF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">build_agent</t>
   </si>
   <si>
     <t xml:space="preserve">USE_AGENT_iterate</t>
@@ -878,7 +896,7 @@
       <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1288,7 +1306,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1722,13 +1740,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -1774,7 +1792,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,7 +1808,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,13 +1864,13 @@
         <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>57</v>
@@ -1906,10 +1924,10 @@
         <v>29</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>32</v>
@@ -1961,15 +1979,12 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2086,67 +2101,112 @@
       <c r="A32" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C32" s="10" t="n">
-        <v>167</v>
+      <c r="B32" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>90</v>
       </c>
       <c r="D32" s="10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E32" s="10" t="n">
         <v>0</v>
       </c>
       <c r="F32" s="0" t="n">
         <f aca="false">SUM(B32:E32)*5</f>
-        <v>1500</v>
+        <v>600</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C33" s="10" t="n">
-        <v>167</v>
+      <c r="B33" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>120</v>
       </c>
       <c r="D33" s="10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E33" s="10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F33" s="0" t="n">
         <f aca="false">SUM(B33:E33)*5</f>
-        <v>1550</v>
+        <v>800</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C34" s="10" t="n">
-        <v>167</v>
+      <c r="B34" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>150</v>
       </c>
       <c r="D34" s="10" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E34" s="10" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F34" s="0" t="n">
         <f aca="false">SUM(B34:E34)*5</f>
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <f aca="false">SUM(B35:E35)*5</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <f aca="false">SUM(B36:E36)*5</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2163,29 +2223,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -2193,15 +2254,15 @@
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>50</v>
@@ -2209,7 +2270,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>40</v>
@@ -2217,7 +2278,7 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>30</v>
@@ -2225,13 +2286,13 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>365</v>
@@ -2251,58 +2312,67 @@
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>75</v>
-      </c>
       <c r="C12" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -2310,7 +2380,7 @@
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -2321,7 +2391,7 @@
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -2330,204 +2400,214 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>585</v>
-      </c>
-      <c r="C21" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>515</v>
+      </c>
+      <c r="C23" s="0" t="n">
         <v>5</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="C28" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B39" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="B40" s="0" t="n">
-        <v>1</v>
+      <c r="C39" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>112</v>
+        <v>115</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>107</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B41" r:id="rId1" display="https://tiled.nsls2.bnl.gov/api/v1/metadata/xpd/sandbox"/>
+    <hyperlink ref="B43" r:id="rId1" display="https://tiled.nsls2.bnl.gov/api/v1/metadata/xpd/sandbox"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2550,7 +2630,7 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.48"/>
@@ -2560,12 +2640,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -2573,15 +2653,15 @@
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>50</v>
@@ -2589,7 +2669,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>40</v>
@@ -2597,7 +2677,7 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>30</v>
@@ -2605,13 +2685,13 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>365</v>
@@ -2631,16 +2711,16 @@
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>14</v>
@@ -2648,41 +2728,41 @@
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>75</v>
-      </c>
       <c r="C12" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -2690,7 +2770,7 @@
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -2698,7 +2778,7 @@
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -2706,15 +2786,15 @@
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -2722,7 +2802,7 @@
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>515</v>
@@ -2733,15 +2813,15 @@
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -2749,39 +2829,39 @@
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -2789,23 +2869,23 @@
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
@@ -2813,31 +2893,31 @@
     </row>
     <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
@@ -2845,7 +2925,7 @@
     </row>
     <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
@@ -2853,10 +2933,10 @@
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2881,7 +2961,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -2892,12 +2972,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -2908,15 +2988,15 @@
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>50</v>
@@ -2924,7 +3004,7 @@
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>40</v>
@@ -2932,7 +3012,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>30</v>
@@ -2940,13 +3020,13 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>365</v>
@@ -3157,7 +3237,7 @@
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>36</v>
@@ -3609,7 +3689,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="78.65"/>
@@ -3618,61 +3698,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3680,7 +3760,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3688,7 +3768,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3696,7 +3776,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3704,7 +3784,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3712,7 +3792,7 @@
         <v>29</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3720,7 +3800,7 @@
         <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3728,7 +3808,7 @@
         <v>38</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3736,7 +3816,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3744,7 +3824,7 @@
         <v>45</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3752,7 +3832,7 @@
         <v>54</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3760,7 +3840,7 @@
         <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3768,7 +3848,7 @@
         <v>54</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3776,7 +3856,7 @@
         <v>53</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3784,7 +3864,7 @@
         <v>53</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3792,7 +3872,7 @@
         <v>53</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3817,7 +3897,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>
@@ -3827,12 +3907,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -3840,15 +3920,15 @@
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>150</v>
@@ -3865,7 +3945,7 @@
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>100</v>
@@ -3882,7 +3962,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>70</v>
@@ -3899,13 +3979,13 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>365</v>
@@ -3942,13 +4022,13 @@
         <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3998,10 +4078,10 @@
         <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4026,7 +4106,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>300</v>
@@ -4045,13 +4125,13 @@
         <v>54</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4059,13 +4139,13 @@
         <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4073,13 +4153,13 @@
         <v>54</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4087,13 +4167,13 @@
         <v>54</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update macros with real data at 1LL09
</commit_message>
<xml_diff>
--- a/scripts/inputs_qserver_kafka_v2.xlsx
+++ b/scripts/inputs_qserver_kafka_v2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="184">
   <si>
     <t xml:space="preserve">Input parameters for tasks in queue server</t>
   </si>
@@ -215,6 +215,15 @@
     <t xml:space="preserve">tcp://localhost:60625</t>
   </si>
   <si>
+    <t xml:space="preserve">Cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ultra1</t>
+  </si>
+  <si>
     <t xml:space="preserve">CsPb(oleate)3_30mM_20240503</t>
   </si>
   <si>
@@ -224,7 +233,28 @@
     <t xml:space="preserve">ZnCl2_60mM_20240701</t>
   </si>
   <si>
-    <t xml:space="preserve">16 ml</t>
+    <t xml:space="preserve">PF_oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plastic_BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35 ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if_wash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wash_loop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wash_sapphire</t>
   </si>
   <si>
     <t xml:space="preserve">Input parameters for data process in kafka</t>
@@ -236,7 +266,7 @@
     <t xml:space="preserve">csv_path</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/20240820_macro_Br</t>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/20240822_macro_Cl</t>
   </si>
   <si>
     <t xml:space="preserve">key_height</t>
@@ -299,7 +329,7 @@
     <t xml:space="preserve">agent_data_path</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/xf28id2/data_post_dilute_100mM_PF</t>
+    <t xml:space="preserve">/home/xf28id2/data_post_dilute_100mM_PF/Cl</t>
   </si>
   <si>
     <t xml:space="preserve">build_agent</t>
@@ -582,8 +612,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -755,7 +786,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -798,6 +829,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -896,7 +935,7 @@
       <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1306,7 +1345,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1740,18 +1779,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="17.83"/>
   </cols>
   <sheetData>
@@ -1819,7 +1858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>11</v>
       </c>
@@ -1830,16 +1869,19 @@
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>16</v>
       </c>
@@ -1850,36 +1892,42 @@
         <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>26</v>
       </c>
@@ -1895,11 +1943,14 @@
       <c r="E15" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>28</v>
       </c>
@@ -1915,27 +1966,33 @@
       <c r="E16" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="F16" s="5" t="n">
+      <c r="F16" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G16" s="5" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1969,10 +2026,10 @@
         <v>37</v>
       </c>
       <c r="B21" s="9" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C21" s="9" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -1981,232 +2038,323 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B26" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>36</v>
+      <c r="C26" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B30" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C30" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D30" s="0" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="D32" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <f aca="false">SUM(B32:E32)*5</f>
-        <v>600</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="D33" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <f aca="false">SUM(B33:E33)*5</f>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="B37" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="D37" s="10" t="n">
+        <v>90</v>
+      </c>
+      <c r="E37" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F37" s="11" t="n">
+        <f aca="false">SUM(B37:E37)/8</f>
+        <v>22.5</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <f aca="false">SUM(B37:E37)*5</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B38" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="D38" s="10" t="n">
+        <v>80</v>
+      </c>
+      <c r="E38" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="F38" s="11" t="n">
+        <f aca="false">SUM(B38:E38)/8</f>
+        <v>22.5</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <f aca="false">SUM(B38:E38)*5</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="D39" s="10" t="n">
+        <v>70</v>
+      </c>
+      <c r="E39" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F39" s="11" t="n">
+        <f aca="false">SUM(B39:E39)/8</f>
+        <v>22.5</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <f aca="false">SUM(B39:E39)*5</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="D40" s="10" t="n">
+        <v>60</v>
+      </c>
+      <c r="E40" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F40" s="11" t="n">
+        <f aca="false">SUM(B40:E40)/8</f>
+        <v>22.5</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <f aca="false">SUM(B40:E40)*5</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="D41" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="C34" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="D34" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="0" t="n">
-        <f aca="false">SUM(B34:E34)*5</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>180</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" s="0" t="n">
-        <f aca="false">SUM(B35:E35)*5</f>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C36" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="D36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <f aca="false">SUM(B36:E36)*5</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E41" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F41" s="11" t="n">
+        <f aca="false">SUM(B41:E41)/8</f>
+        <v>22.5</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <f aca="false">SUM(B41:E41)*5</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="11"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="11"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="11"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2225,28 +2373,28 @@
   </sheetPr>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -2254,15 +2402,15 @@
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>50</v>
@@ -2270,7 +2418,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>40</v>
@@ -2278,7 +2426,7 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>30</v>
@@ -2286,21 +2434,21 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>365</v>
       </c>
-      <c r="E8" s="11" t="n">
+      <c r="E8" s="13" t="n">
         <v>0.360936</v>
       </c>
-      <c r="F8" s="11" t="n">
+      <c r="F8" s="13" t="n">
         <v>952628</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -2312,16 +2460,16 @@
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>14</v>
@@ -2332,47 +2480,47 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -2380,7 +2528,7 @@
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -2391,7 +2539,7 @@
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -2403,7 +2551,7 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -2411,15 +2559,15 @@
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
@@ -2428,7 +2576,7 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -2436,7 +2584,7 @@
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>515</v>
@@ -2447,7 +2595,7 @@
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -2455,48 +2603,48 @@
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>0</v>
@@ -2504,23 +2652,23 @@
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>0</v>
@@ -2528,37 +2676,37 @@
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>0</v>
@@ -2566,7 +2714,7 @@
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
@@ -2574,35 +2722,35 @@
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>118</v>
+        <v>127</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2630,7 +2778,7 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.48"/>
@@ -2640,12 +2788,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -2653,15 +2801,15 @@
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>50</v>
@@ -2669,7 +2817,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>40</v>
@@ -2677,7 +2825,7 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>30</v>
@@ -2685,21 +2833,21 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>365</v>
       </c>
-      <c r="E8" s="11" t="n">
+      <c r="E8" s="13" t="n">
         <v>0.360936</v>
       </c>
-      <c r="F8" s="11" t="n">
+      <c r="F8" s="13" t="n">
         <v>952628</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -2711,16 +2859,16 @@
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>14</v>
@@ -2728,41 +2876,41 @@
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -2770,7 +2918,7 @@
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -2778,7 +2926,7 @@
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -2786,15 +2934,15 @@
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -2802,7 +2950,7 @@
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>515</v>
@@ -2813,15 +2961,15 @@
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -2829,39 +2977,39 @@
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -2869,23 +3017,23 @@
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
@@ -2893,31 +3041,31 @@
     </row>
     <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>0</v>
@@ -2925,7 +3073,7 @@
     </row>
     <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>0</v>
@@ -2933,10 +3081,10 @@
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2961,7 +3109,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -2972,12 +3120,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -2988,15 +3136,15 @@
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>50</v>
@@ -3004,7 +3152,7 @@
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>40</v>
@@ -3012,7 +3160,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>30</v>
@@ -3020,21 +3168,21 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>365</v>
       </c>
-      <c r="E7" s="11" t="n">
+      <c r="E7" s="13" t="n">
         <v>0.360936</v>
       </c>
-      <c r="F7" s="11" t="n">
+      <c r="F7" s="13" t="n">
         <v>952628</v>
       </c>
       <c r="G7" s="0" t="n">
@@ -3237,7 +3385,7 @@
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>36</v>
@@ -3689,7 +3837,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="78.65"/>
@@ -3698,61 +3846,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>140</v>
+        <v>147</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3760,7 +3908,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3768,7 +3916,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3776,7 +3924,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3784,7 +3932,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3792,7 +3940,7 @@
         <v>29</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3800,7 +3948,7 @@
         <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3808,7 +3956,7 @@
         <v>38</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3816,7 +3964,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3824,7 +3972,7 @@
         <v>45</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3832,7 +3980,7 @@
         <v>54</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3840,7 +3988,7 @@
         <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3848,7 +3996,7 @@
         <v>54</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3856,7 +4004,7 @@
         <v>53</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3864,7 +4012,7 @@
         <v>53</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3872,7 +4020,7 @@
         <v>53</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -3897,7 +4045,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>
@@ -3907,12 +4055,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -3920,15 +4068,15 @@
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>150</v>
@@ -3945,7 +4093,7 @@
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>100</v>
@@ -3962,7 +4110,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>70</v>
@@ -3979,13 +4127,13 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>365</v>
@@ -4022,13 +4170,13 @@
         <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4078,10 +4226,10 @@
         <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4106,7 +4254,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>300</v>
@@ -4125,13 +4273,13 @@
         <v>54</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4139,13 +4287,13 @@
         <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4153,13 +4301,13 @@
         <v>54</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4167,13 +4315,13 @@
         <v>54</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add wait=True to count_stream
</commit_message>
<xml_diff>
--- a/scripts/inputs_qserver_kafka_v2.xlsx
+++ b/scripts/inputs_qserver_kafka_v2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="184">
   <si>
     <t xml:space="preserve">Input parameters for tasks in queue server</t>
   </si>
@@ -230,7 +230,7 @@
     <t xml:space="preserve">TOABr_100mM_20240814</t>
   </si>
   <si>
-    <t xml:space="preserve">ZnCl2_60mM_20240701</t>
+    <t xml:space="preserve">ZnCl2_60mM_20240731</t>
   </si>
   <si>
     <t xml:space="preserve">PF_oil</t>
@@ -239,13 +239,13 @@
     <t xml:space="preserve">plastic_BD</t>
   </si>
   <si>
-    <t xml:space="preserve">35 ml</t>
+    <t xml:space="preserve">10 ml</t>
   </si>
   <si>
     <t xml:space="preserve">25 ml</t>
   </si>
   <si>
-    <t xml:space="preserve">10 ml</t>
+    <t xml:space="preserve">17 ml</t>
   </si>
   <si>
     <t xml:space="preserve">if_wash</t>
@@ -266,7 +266,7 @@
     <t xml:space="preserve">csv_path</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/20240822_macro_Cl</t>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/20240829_macro_Cl</t>
   </si>
   <si>
     <t xml:space="preserve">key_height</t>
@@ -612,9 +612,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -786,7 +787,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -831,12 +832,16 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -931,11 +936,11 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1345,7 +1350,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
@@ -1779,13 +1784,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -1799,6 +1804,7 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>1</v>
@@ -1815,6 +1821,7 @@
         <v>61</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>5</v>
@@ -1842,6 +1849,7 @@
         <v>8</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>9</v>
@@ -1978,10 +1986,10 @@
         <v>29</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>71</v>
@@ -1996,6 +2004,7 @@
         <v>31</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>33</v>
@@ -2026,10 +2035,10 @@
         <v>37</v>
       </c>
       <c r="B21" s="9" t="n">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C21" s="9" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -2061,7 +2070,7 @@
         <v>42</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>19</v>
@@ -2084,7 +2093,6 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>38</v>
@@ -2101,10 +2109,10 @@
         <v>45</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,7 +2151,6 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>52</v>
@@ -2181,36 +2188,76 @@
       <c r="I34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="11"/>
+      <c r="A35" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="11" t="n">
+        <v>72.85</v>
+      </c>
+      <c r="C35" s="11" t="n">
+        <v>218.55</v>
+      </c>
+      <c r="D35" s="11" t="n">
+        <v>21.86</v>
+      </c>
+      <c r="E35" s="11" t="n">
+        <v>46.75</v>
+      </c>
+      <c r="F35" s="12" t="n">
+        <f aca="false">SUM(B35:E35)/9</f>
+        <v>40.0011111111111</v>
+      </c>
+      <c r="G35" s="13" t="n">
+        <f aca="false">SUM(B35:E35)*5</f>
+        <v>1800.05</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="11"/>
+      <c r="A36" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="11" t="n">
+        <v>21.18</v>
+      </c>
+      <c r="C36" s="11" t="n">
+        <v>63.53</v>
+      </c>
+      <c r="D36" s="11" t="n">
+        <v>95.3</v>
+      </c>
+      <c r="E36" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="12" t="n">
+        <f aca="false">SUM(B36:E36)/9</f>
+        <v>20.0011111111111</v>
+      </c>
+      <c r="G36" s="13" t="n">
+        <f aca="false">SUM(B36:E36)*5</f>
+        <v>900.05</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="11" t="n">
+        <v>25.31</v>
+      </c>
+      <c r="C37" s="11" t="n">
+        <v>75.93</v>
+      </c>
+      <c r="D37" s="11" t="n">
+        <v>75.93</v>
+      </c>
+      <c r="E37" s="11" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="F37" s="12" t="n">
+        <f aca="false">SUM(B37:E37)/9</f>
         <v>20</v>
       </c>
-      <c r="C37" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="D37" s="10" t="n">
-        <v>90</v>
-      </c>
-      <c r="E37" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F37" s="11" t="n">
-        <f aca="false">SUM(B37:E37)/8</f>
-        <v>22.5</v>
-      </c>
-      <c r="G37" s="0" t="n">
+      <c r="G37" s="13" t="n">
         <f aca="false">SUM(B37:E37)*5</f>
         <v>900</v>
       </c>
@@ -2219,48 +2266,48 @@
       <c r="A38" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="C38" s="0" t="n">
-        <v>66</v>
-      </c>
-      <c r="D38" s="10" t="n">
-        <v>80</v>
-      </c>
-      <c r="E38" s="10" t="n">
-        <v>12</v>
-      </c>
-      <c r="F38" s="11" t="n">
-        <f aca="false">SUM(B38:E38)/8</f>
-        <v>22.5</v>
-      </c>
-      <c r="G38" s="0" t="n">
+      <c r="B38" s="11" t="n">
+        <v>31.43</v>
+      </c>
+      <c r="C38" s="11" t="n">
+        <v>94.29</v>
+      </c>
+      <c r="D38" s="11" t="n">
+        <v>47.15</v>
+      </c>
+      <c r="E38" s="11" t="n">
+        <v>7.14</v>
+      </c>
+      <c r="F38" s="12" t="n">
+        <f aca="false">SUM(B38:E38)/9</f>
+        <v>20.0011111111111</v>
+      </c>
+      <c r="G38" s="13" t="n">
         <f aca="false">SUM(B38:E38)*5</f>
-        <v>900</v>
+        <v>900.05</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="C39" s="0" t="n">
-        <v>75</v>
-      </c>
-      <c r="D39" s="10" t="n">
-        <v>70</v>
-      </c>
-      <c r="E39" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F39" s="11" t="n">
-        <f aca="false">SUM(B39:E39)/8</f>
-        <v>22.5</v>
-      </c>
-      <c r="G39" s="0" t="n">
+      <c r="B39" s="11" t="n">
+        <v>35.75</v>
+      </c>
+      <c r="C39" s="11" t="n">
+        <v>107.25</v>
+      </c>
+      <c r="D39" s="11" t="n">
+        <v>26.81</v>
+      </c>
+      <c r="E39" s="11" t="n">
+        <v>10.19</v>
+      </c>
+      <c r="F39" s="12" t="n">
+        <f aca="false">SUM(B39:E39)/9</f>
+        <v>20</v>
+      </c>
+      <c r="G39" s="13" t="n">
         <f aca="false">SUM(B39:E39)*5</f>
         <v>900</v>
       </c>
@@ -2269,92 +2316,60 @@
       <c r="A40" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <v>84</v>
-      </c>
-      <c r="D40" s="10" t="n">
-        <v>60</v>
-      </c>
-      <c r="E40" s="10" t="n">
-        <v>8</v>
-      </c>
-      <c r="F40" s="11" t="n">
-        <f aca="false">SUM(B40:E40)/8</f>
-        <v>22.5</v>
-      </c>
-      <c r="G40" s="0" t="n">
+      <c r="B40" s="11" t="n">
+        <v>38.96</v>
+      </c>
+      <c r="C40" s="11" t="n">
+        <v>116.88</v>
+      </c>
+      <c r="D40" s="11" t="n">
+        <v>11.69</v>
+      </c>
+      <c r="E40" s="11" t="n">
+        <v>12.47</v>
+      </c>
+      <c r="F40" s="12" t="n">
+        <f aca="false">SUM(B40:E40)/9</f>
+        <v>20</v>
+      </c>
+      <c r="G40" s="13" t="n">
         <f aca="false">SUM(B40:E40)*5</f>
         <v>900</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="C41" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="D41" s="10" t="n">
-        <v>50</v>
-      </c>
-      <c r="E41" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F41" s="11" t="n">
-        <f aca="false">SUM(B41:E41)/8</f>
-        <v>22.5</v>
-      </c>
-      <c r="G41" s="0" t="n">
-        <f aca="false">SUM(B41:E41)*5</f>
-        <v>900</v>
-      </c>
-    </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="12"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
       <c r="E43" s="10"/>
-      <c r="F43" s="11"/>
+      <c r="F43" s="12"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="11"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2374,10 +2389,10 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
@@ -2445,10 +2460,10 @@
       <c r="D8" s="0" t="n">
         <v>365</v>
       </c>
-      <c r="E8" s="13" t="n">
+      <c r="E8" s="14" t="n">
         <v>0.360936</v>
       </c>
-      <c r="F8" s="13" t="n">
+      <c r="F8" s="14" t="n">
         <v>952628</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -2724,7 +2739,7 @@
       <c r="A43" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="15" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2778,7 +2793,7 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.48"/>
@@ -2844,10 +2859,10 @@
       <c r="D8" s="0" t="n">
         <v>365</v>
       </c>
-      <c r="E8" s="13" t="n">
+      <c r="E8" s="14" t="n">
         <v>0.360936</v>
       </c>
-      <c r="F8" s="13" t="n">
+      <c r="F8" s="14" t="n">
         <v>952628</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -3109,7 +3124,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -3179,10 +3194,10 @@
       <c r="D7" s="0" t="n">
         <v>365</v>
       </c>
-      <c r="E7" s="13" t="n">
+      <c r="E7" s="14" t="n">
         <v>0.360936</v>
       </c>
-      <c r="F7" s="13" t="n">
+      <c r="F7" s="14" t="n">
         <v>952628</v>
       </c>
       <c r="G7" s="0" t="n">
@@ -3837,7 +3852,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="78.65"/>
@@ -3848,7 +3863,7 @@
       <c r="A1" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4045,7 +4060,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>

</xml_diff>

<commit_message>
Update workflow v2 for XPD
</commit_message>
<xml_diff>
--- a/scripts/inputs_qserver_kafka_v2.xlsx
+++ b/scripts/inputs_qserver_kafka_v2.xlsx
@@ -5,14 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="qserver_test" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="qserver_XPD" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="qserver_1LL09" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="kafka_process" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="kafka_process (2)" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="kafka_test" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="qserver_XPD" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="qserver_1LL09" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="kafka_process" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="inputs" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="detail of variables" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="example1" sheetId="8" state="visible" r:id="rId9"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="170">
   <si>
     <t xml:space="preserve">Input parameters for tasks in queue server</t>
   </si>
@@ -86,394 +86,352 @@
     <t xml:space="preserve">dds2_p2</t>
   </si>
   <si>
+    <t xml:space="preserve">dds3_p2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dds3_p1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">precursor_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CsPb(oleate)3_30mM_20240216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOABr_66mM_20240430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZnCl2_60mM_20240513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toluene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">syringe_mater_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">syringe_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target_vol_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CsPb_010_Br_131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CsPb_012_Br_142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CsPb_010_Br_166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait_dilute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if_wash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wash_loop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 ul/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 ul/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mixer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60 cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resident_t_ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate_unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ul/min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uvvis_config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qepro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perkin_config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pe1c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auto_set_target_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set_target_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infuse_rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input parameters for data process in kafka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy_kafka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csv_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/20240911_v2_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">key_height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLQY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quinine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate_label_dic_key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CsPb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZnI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate_label_dic_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infusion_rate_CsPb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infusion_rate_Br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infusion_rate_I2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infusion_rate_Cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new_points_label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use_good_bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post_dilute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix_Br_ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write_agent_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agent_data_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/agent_data/test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">build_agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use_1st_prediction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USE_AGENT_iterate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peak_target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iq_to_gr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iq_to_gr_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/pdfstream_test/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cfg_fn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pdfgetx3.cfg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bkg_fn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**bkg**.chi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iq_fn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**CsPb**.chi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search_and_match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mystery_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/pdffit2_example/CsPbBr3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/pdffit2_example/results_CsPbBr_chemsys_search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fitting_pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fitting_pdf_path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/pdffit2_example/CsPbBr3/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cif_fn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CsPbBr3_Orthorhombic.cif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gr_fn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CsPbBr3.gr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy_pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write_to_sandbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sandbox_uri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://tiled.nsls2.bnl.gov/api/v1/metadata/xpd/sandbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beamline_acronym</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fn_TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OAm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dds1_p1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ultra1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CsPb(oleate)3_30mM_20240802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOABr_100mM_20240828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZnCl2_60mM_20240731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OAm_Tol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF_oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plastic_BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35 ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ultra2</t>
+  </si>
+  <si>
     <t xml:space="preserve">dds1_p2</t>
   </si>
   <si>
-    <t xml:space="preserve">dds3_p1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">precursor_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CsPb(oleate)3_30mM_20240216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOABr_66mM_20240430</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZnCl2_60mM_20240513</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toluene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">syringe_mater_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">steel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">syringe_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">target_vol_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40 ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sample</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CsPb_010_Br_131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CsPb_012_Br_142</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CsPb_010_Br_166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait_dilute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mixer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60 cm</t>
+    <t xml:space="preserve">det</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp://localhost:60615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp://localhost:60625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/20240902_macro_Cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infusion_rate_OAm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/xf28id2/data_post_dilute_100mM_PF/Cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input parameters for tasks in queue and kafka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/20240614_dilute_OAm</t>
   </si>
   <si>
     <t xml:space="preserve">wash_tube</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200 ul/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dds1_p1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 ul/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resident_t_ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rate_unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ul/min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uvvis_config</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qepro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">perkin_config</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pe2c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">auto_set_target_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set_target_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infuse_rates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OAm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dds3_p2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OAm_Tol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ultra2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">det</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tcp://localhost:60615</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tcp://localhost:60625</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ultra1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CsPb(oleate)3_30mM_20240503</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOABr_100mM_20240814</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZnCl2_60mM_20240731</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PF_oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plastic_BD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if_wash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wash_loop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wash_sapphire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input parameters for data process in kafka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dummy_kafka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">csv_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/20240829_macro_Cl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">key_height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLQY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quinine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rate_label_dic_key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CsPb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZnI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rate_label_dic_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infusion_rate_CsPb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infusion_rate_Br</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infusion_rate_I2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infusion_rate_Cl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infusion_rate_OAm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">new_points_label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">use_good_bad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">post_dilute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fix_Br_ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">write_agent_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">agent_data_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/xf28id2/data_post_dilute_100mM_PF/Cl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">build_agent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USE_AGENT_iterate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">peak_target</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iq_to_gr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iq_to_gr_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/pdfstream_test/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cfg_fn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pdfgetx3.cfg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bkg_fn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**bkg**.chi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iq_fn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**CsPb**.chi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search_and_match</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mystery_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/pdffit2_example/CsPbBr3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/pdffit2_example/results_CsPbBr_chemsys_search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fitting_pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fitting_pdf_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/pdffit2_example/CsPbBr3/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cif_fn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CsPbBr3_Orthorhombic.cif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gr_fn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CsPbBr3.gr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dummy_pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">write_to_sandbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sandbox_uri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://tiled.nsls2.bnl.gov/api/v1/metadata/xpd/sandbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beamline_acronym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fn_TBD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/20240614_dilute_OAm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/202405_halide_data/with_xray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">agent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">build_agen(peak_target=peak_target, agent_data_path=agent_data_path)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gr_path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/home/xf28id2/Documents/ChengHung/pdfstream_test/pdfgetx3.cfg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glob.glob(os.path.join(gr_path, '**CsPb**.chi'))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glob.glob(os.path.join(gr_path, '**bkg**.chi'))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pdf_cif_dir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cif_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">os.path.join(pdf_cif_dir, 'CsPbBr3_Orthorhombic.cif')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gr_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">os.path.join(pdf_cif_dir, 'CsPbBr3.gr')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">use_sandbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sandbox_tiled_client</t>
-  </si>
-  <si>
-    <t xml:space="preserve">from_uri("https://tiled.nsls2.bnl.gov/api/v1/metadata/xpd/sandbox")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input parameters for tasks in queue and kafka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dummy_test</t>
   </si>
   <si>
     <t xml:space="preserve">num_uvvis</t>
@@ -612,10 +570,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
-    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -787,7 +746,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -828,20 +787,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -934,19 +897,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L46" activeCellId="0" sqref="L46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="17.83"/>
   </cols>
   <sheetData>
@@ -955,6 +917,7 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>1</v>
@@ -971,6 +934,7 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>5</v>
@@ -987,7 +951,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1116,7 +1080,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>33</v>
       </c>
@@ -1130,23 +1094,19 @@
         <v>36</v>
       </c>
       <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="9" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C21" s="9" t="n">
         <v>5</v>
@@ -1156,178 +1116,242 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
-    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>40</v>
+      <c r="B22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="0" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="G23" s="0" t="s">
+      <c r="B26" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="C26" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B30" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C30" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D30" s="10" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C32" s="10" t="n">
-        <v>167</v>
-      </c>
-      <c r="D32" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <f aca="false">SUM(B32:D32)*5</f>
-        <v>1500</v>
+        <v>52</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C33" s="10" t="n">
-        <v>167</v>
-      </c>
-      <c r="D33" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <f aca="false">SUM(B33:D33)*5</f>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="B35" s="11" t="n">
+        <v>39.62</v>
+      </c>
+      <c r="C35" s="11" t="n">
+        <v>118.86</v>
+      </c>
+      <c r="D35" s="11" t="n">
+        <v>178.29</v>
+      </c>
+      <c r="E35" s="11" t="n">
+        <v>23.23</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="13"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C34" s="10" t="n">
-        <v>167</v>
-      </c>
-      <c r="D34" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <f aca="false">SUM(B34:D34)*5</f>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B36" s="11" t="n">
+        <v>47.32</v>
+      </c>
+      <c r="C36" s="11" t="n">
+        <v>141.96</v>
+      </c>
+      <c r="D36" s="11" t="n">
+        <v>141.96</v>
+      </c>
+      <c r="E36" s="11" t="n">
+        <v>28.76</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="13"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="11" t="n">
+        <v>58.76</v>
+      </c>
+      <c r="C37" s="11" t="n">
+        <v>176.28</v>
+      </c>
+      <c r="D37" s="11" t="n">
+        <v>88.14</v>
+      </c>
+      <c r="E37" s="11" t="n">
+        <v>36.82</v>
+      </c>
+      <c r="F37" s="12"/>
+      <c r="G37" s="13"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1344,437 +1368,397 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>4</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>8</v>
+        <v>62</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>365</v>
+      </c>
+      <c r="E8" s="15" t="n">
+        <v>0.360936</v>
+      </c>
+      <c r="F8" s="15" t="n">
+        <v>952628</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>1.337</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.546</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>20</v>
+        <v>72</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>25</v>
+        <v>73</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>27</v>
+        <v>74</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="4" t="n">
-        <v>50</v>
+        <v>75</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="F16" s="5" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+        <v>77</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="9" t="n">
-        <v>30</v>
-      </c>
-      <c r="C21" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>40</v>
+        <v>80</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <v>360</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>2</v>
+        <v>515</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C32" s="10" t="n">
-        <v>167</v>
-      </c>
-      <c r="D32" s="10" t="n">
+    </row>
+    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <f aca="false">SUM(B32:E32)*5</f>
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C33" s="10" t="n">
-        <v>167</v>
-      </c>
-      <c r="D33" s="10" t="n">
+      <c r="B39" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="E33" s="10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <f aca="false">SUM(B33:E33)*5</f>
-        <v>1550</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="10" t="n">
-        <v>33</v>
-      </c>
-      <c r="C34" s="10" t="n">
-        <v>167</v>
-      </c>
-      <c r="D34" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="E34" s="10" t="n">
-        <v>20</v>
-      </c>
-      <c r="F34" s="0" t="n">
-        <f aca="false">SUM(B34:E34)*5</f>
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F47" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B44" r:id="rId1" display="https://tiled.nsls2.bnl.gov/api/v1/metadata/xpd/sandbox"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
@@ -1786,11 +1770,11 @@
   </sheetPr>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -1810,7 +1794,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,7 +1802,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1877,13 +1861,13 @@
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>15</v>
@@ -1903,13 +1887,13 @@
         <v>20</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,19 +1901,19 @@
         <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>57</v>
+        <v>118</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>25</v>
@@ -1952,7 +1936,7 @@
         <v>27</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>27</v>
@@ -1986,19 +1970,19 @@
         <v>29</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>31</v>
@@ -2047,7 +2031,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -2058,50 +2042,36 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>50</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>20</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2142,7 +2112,7 @@
         <v>50</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>0.2</v>
@@ -2192,24 +2162,24 @@
         <v>54</v>
       </c>
       <c r="B35" s="11" t="n">
-        <v>72.85</v>
+        <v>39.62</v>
       </c>
       <c r="C35" s="11" t="n">
-        <v>218.55</v>
+        <v>118.86</v>
       </c>
       <c r="D35" s="11" t="n">
-        <v>21.86</v>
+        <v>178.29</v>
       </c>
       <c r="E35" s="11" t="n">
-        <v>46.75</v>
+        <v>23.23</v>
       </c>
       <c r="F35" s="12" t="n">
         <f aca="false">SUM(B35:E35)/9</f>
-        <v>40.0011111111111</v>
+        <v>40</v>
       </c>
       <c r="G35" s="13" t="n">
         <f aca="false">SUM(B35:E35)*5</f>
-        <v>1800.05</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2217,24 +2187,24 @@
         <v>54</v>
       </c>
       <c r="B36" s="11" t="n">
-        <v>21.18</v>
+        <v>47.32</v>
       </c>
       <c r="C36" s="11" t="n">
-        <v>63.53</v>
+        <v>141.96</v>
       </c>
       <c r="D36" s="11" t="n">
-        <v>95.3</v>
+        <v>141.96</v>
       </c>
       <c r="E36" s="11" t="n">
-        <v>0</v>
+        <v>28.76</v>
       </c>
       <c r="F36" s="12" t="n">
         <f aca="false">SUM(B36:E36)/9</f>
-        <v>20.0011111111111</v>
+        <v>40</v>
       </c>
       <c r="G36" s="13" t="n">
         <f aca="false">SUM(B36:E36)*5</f>
-        <v>900.05</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,24 +2212,24 @@
         <v>54</v>
       </c>
       <c r="B37" s="11" t="n">
-        <v>25.31</v>
+        <v>58.76</v>
       </c>
       <c r="C37" s="11" t="n">
-        <v>75.93</v>
+        <v>176.28</v>
       </c>
       <c r="D37" s="11" t="n">
-        <v>75.93</v>
+        <v>88.14</v>
       </c>
       <c r="E37" s="11" t="n">
-        <v>2.83</v>
+        <v>36.82</v>
       </c>
       <c r="F37" s="12" t="n">
         <f aca="false">SUM(B37:E37)/9</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G37" s="13" t="n">
         <f aca="false">SUM(B37:E37)*5</f>
-        <v>900</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,24 +2237,24 @@
         <v>54</v>
       </c>
       <c r="B38" s="11" t="n">
-        <v>31.43</v>
+        <v>66.85</v>
       </c>
       <c r="C38" s="11" t="n">
-        <v>94.29</v>
+        <v>200.55</v>
       </c>
       <c r="D38" s="11" t="n">
-        <v>47.15</v>
+        <v>50.14</v>
       </c>
       <c r="E38" s="11" t="n">
-        <v>7.14</v>
+        <v>42.46</v>
       </c>
       <c r="F38" s="12" t="n">
         <f aca="false">SUM(B38:E38)/9</f>
-        <v>20.0011111111111</v>
+        <v>40</v>
       </c>
       <c r="G38" s="13" t="n">
         <f aca="false">SUM(B38:E38)*5</f>
-        <v>900.05</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2292,50 +2262,33 @@
         <v>54</v>
       </c>
       <c r="B39" s="11" t="n">
-        <v>35.75</v>
+        <v>72.85</v>
       </c>
       <c r="C39" s="11" t="n">
-        <v>107.25</v>
+        <v>218.55</v>
       </c>
       <c r="D39" s="11" t="n">
-        <v>26.81</v>
+        <v>21.86</v>
       </c>
       <c r="E39" s="11" t="n">
-        <v>10.19</v>
+        <v>46.75</v>
       </c>
       <c r="F39" s="12" t="n">
         <f aca="false">SUM(B39:E39)/9</f>
-        <v>20</v>
+        <v>40.0011111111111</v>
       </c>
       <c r="G39" s="13" t="n">
         <f aca="false">SUM(B39:E39)*5</f>
-        <v>900</v>
+        <v>1800.05</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="11" t="n">
-        <v>38.96</v>
-      </c>
-      <c r="C40" s="11" t="n">
-        <v>116.88</v>
-      </c>
-      <c r="D40" s="11" t="n">
-        <v>11.69</v>
-      </c>
-      <c r="E40" s="11" t="n">
-        <v>12.47</v>
-      </c>
-      <c r="F40" s="12" t="n">
-        <f aca="false">SUM(B40:E40)/9</f>
-        <v>20</v>
-      </c>
-      <c r="G40" s="13" t="n">
-        <f aca="false">SUM(B40:E40)*5</f>
-        <v>900</v>
-      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="11"/>
@@ -2349,7 +2302,7 @@
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
-      <c r="E43" s="10"/>
+      <c r="E43" s="14"/>
       <c r="F43" s="12"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2386,13 +2339,584 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:I46"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="17.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="9" t="n">
+        <v>30</v>
+      </c>
+      <c r="C21" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="11" t="n">
+        <v>39.62</v>
+      </c>
+      <c r="C35" s="11" t="n">
+        <v>118.86</v>
+      </c>
+      <c r="D35" s="11" t="n">
+        <v>178.29</v>
+      </c>
+      <c r="E35" s="11" t="n">
+        <v>23.23</v>
+      </c>
+      <c r="F35" s="12" t="n">
+        <f aca="false">SUM(B35:E35)/9</f>
+        <v>40</v>
+      </c>
+      <c r="G35" s="13" t="n">
+        <f aca="false">SUM(B35:E35)*5</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="11" t="n">
+        <v>47.32</v>
+      </c>
+      <c r="C36" s="11" t="n">
+        <v>141.96</v>
+      </c>
+      <c r="D36" s="11" t="n">
+        <v>141.96</v>
+      </c>
+      <c r="E36" s="11" t="n">
+        <v>28.76</v>
+      </c>
+      <c r="F36" s="12" t="n">
+        <f aca="false">SUM(B36:E36)/9</f>
+        <v>40</v>
+      </c>
+      <c r="G36" s="13" t="n">
+        <f aca="false">SUM(B36:E36)*5</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="11" t="n">
+        <v>58.76</v>
+      </c>
+      <c r="C37" s="11" t="n">
+        <v>176.28</v>
+      </c>
+      <c r="D37" s="11" t="n">
+        <v>88.14</v>
+      </c>
+      <c r="E37" s="11" t="n">
+        <v>36.82</v>
+      </c>
+      <c r="F37" s="12" t="n">
+        <f aca="false">SUM(B37:E37)/9</f>
+        <v>40</v>
+      </c>
+      <c r="G37" s="13" t="n">
+        <f aca="false">SUM(B37:E37)*5</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="11" t="n">
+        <v>66.85</v>
+      </c>
+      <c r="C38" s="11" t="n">
+        <v>200.55</v>
+      </c>
+      <c r="D38" s="11" t="n">
+        <v>50.14</v>
+      </c>
+      <c r="E38" s="11" t="n">
+        <v>42.46</v>
+      </c>
+      <c r="F38" s="12" t="n">
+        <f aca="false">SUM(B38:E38)/9</f>
+        <v>40</v>
+      </c>
+      <c r="G38" s="13" t="n">
+        <f aca="false">SUM(B38:E38)*5</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="11" t="n">
+        <v>72.85</v>
+      </c>
+      <c r="C39" s="11" t="n">
+        <v>218.55</v>
+      </c>
+      <c r="D39" s="11" t="n">
+        <v>21.86</v>
+      </c>
+      <c r="E39" s="11" t="n">
+        <v>46.75</v>
+      </c>
+      <c r="F39" s="12" t="n">
+        <f aca="false">SUM(B39:E39)/9</f>
+        <v>40.0011111111111</v>
+      </c>
+      <c r="G39" s="13" t="n">
+        <f aca="false">SUM(B39:E39)*5</f>
+        <v>1800.05</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
@@ -2404,28 +2928,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>50</v>
@@ -2433,7 +2957,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>40</v>
@@ -2441,7 +2965,7 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>30</v>
@@ -2449,21 +2973,21 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>365</v>
       </c>
-      <c r="E8" s="14" t="n">
+      <c r="E8" s="15" t="n">
         <v>0.360936</v>
       </c>
-      <c r="F8" s="14" t="n">
+      <c r="F8" s="15" t="n">
         <v>952628</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -2475,67 +2999,67 @@
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -2543,7 +3067,7 @@
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -2554,7 +3078,7 @@
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -2566,7 +3090,7 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -2574,24 +3098,24 @@
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -2599,510 +3123,187 @@
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B23" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="0" t="n">
         <v>515</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C24" s="0" t="n">
         <v>5</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>106</v>
+        <v>83</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>0</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>115</v>
+        <v>92</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>0</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>120</v>
+        <v>97</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="B41" s="0" t="n">
-        <v>0</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>128</v>
+        <v>105</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="B46" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="0" t="s">
+    </row>
+    <row r="45" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>123</v>
+      <c r="B47" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B43" r:id="rId1" display="https://tiled.nsls2.bnl.gov/api/v1/metadata/xpd/sandbox"/>
+    <hyperlink ref="B44" r:id="rId1" display="https://tiled.nsls2.bnl.gov/api/v1/metadata/xpd/sandbox"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H40"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="13.66"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>365</v>
-      </c>
-      <c r="E8" s="14" t="n">
-        <v>0.360936</v>
-      </c>
-      <c r="F8" s="14" t="n">
-        <v>952628</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>1.337</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>0.546</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>515</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B38" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="B39" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3124,7 +3325,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.83"/>
@@ -3135,12 +3336,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -3151,15 +3352,15 @@
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>50</v>
@@ -3167,7 +3368,7 @@
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>40</v>
@@ -3175,7 +3376,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>30</v>
@@ -3183,21 +3384,21 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>365</v>
       </c>
-      <c r="E7" s="14" t="n">
+      <c r="E7" s="15" t="n">
         <v>0.360936</v>
       </c>
-      <c r="F7" s="14" t="n">
+      <c r="F7" s="15" t="n">
         <v>952628</v>
       </c>
       <c r="G7" s="0" t="n">
@@ -3224,7 +3425,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>15</v>
@@ -3241,10 +3442,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>56</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>20</v>
@@ -3264,7 +3465,7 @@
         <v>24</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>57</v>
+        <v>118</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>25</v>
@@ -3349,18 +3550,18 @@
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -3369,19 +3570,19 @@
         <v>50</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>20</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>360</v>
@@ -3400,7 +3601,7 @@
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>36</v>
@@ -3421,16 +3622,16 @@
       <c r="A20" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="10" t="n">
+      <c r="B20" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="C20" s="10" t="n">
+      <c r="C20" s="14" t="n">
         <v>167</v>
       </c>
-      <c r="D20" s="10" t="n">
+      <c r="D20" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="E20" s="10" t="n">
+      <c r="E20" s="14" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="0" t="n">
@@ -3445,16 +3646,16 @@
       <c r="A21" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="10" t="n">
+      <c r="B21" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="C21" s="10" t="n">
+      <c r="C21" s="14" t="n">
         <v>167</v>
       </c>
-      <c r="D21" s="10" t="n">
+      <c r="D21" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="E21" s="10" t="n">
+      <c r="E21" s="14" t="n">
         <v>10</v>
       </c>
       <c r="F21" s="0" t="n">
@@ -3466,16 +3667,16 @@
       <c r="A22" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="10" t="n">
+      <c r="B22" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="C22" s="10" t="n">
+      <c r="C22" s="14" t="n">
         <v>167</v>
       </c>
-      <c r="D22" s="10" t="n">
+      <c r="D22" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="E22" s="10" t="n">
+      <c r="E22" s="14" t="n">
         <v>20</v>
       </c>
       <c r="F22" s="0" t="n">
@@ -3487,16 +3688,16 @@
       <c r="A23" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="10" t="n">
+      <c r="B23" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="C23" s="10" t="n">
+      <c r="C23" s="14" t="n">
         <v>167</v>
       </c>
-      <c r="D23" s="10" t="n">
+      <c r="D23" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="E23" s="10" t="n">
+      <c r="E23" s="14" t="n">
         <v>30</v>
       </c>
       <c r="F23" s="0" t="n">
@@ -3508,16 +3709,16 @@
       <c r="A24" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="10" t="n">
+      <c r="B24" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="C24" s="10" t="n">
+      <c r="C24" s="14" t="n">
         <v>167</v>
       </c>
-      <c r="D24" s="10" t="n">
+      <c r="D24" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="E24" s="10" t="n">
+      <c r="E24" s="14" t="n">
         <v>40</v>
       </c>
       <c r="F24" s="0" t="n">
@@ -3529,16 +3730,16 @@
       <c r="A25" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="10" t="n">
+      <c r="B25" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="C25" s="10" t="n">
+      <c r="C25" s="14" t="n">
         <v>167</v>
       </c>
-      <c r="D25" s="10" t="n">
+      <c r="D25" s="14" t="n">
         <v>140</v>
       </c>
-      <c r="E25" s="10" t="n">
+      <c r="E25" s="14" t="n">
         <v>0</v>
       </c>
       <c r="F25" s="0" t="n">
@@ -3550,16 +3751,16 @@
       <c r="A26" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="10" t="n">
+      <c r="B26" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="C26" s="10" t="n">
+      <c r="C26" s="14" t="n">
         <v>167</v>
       </c>
-      <c r="D26" s="10" t="n">
+      <c r="D26" s="14" t="n">
         <v>130</v>
       </c>
-      <c r="E26" s="10" t="n">
+      <c r="E26" s="14" t="n">
         <v>10</v>
       </c>
       <c r="F26" s="0" t="n">
@@ -3571,16 +3772,16 @@
       <c r="A27" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="10" t="n">
+      <c r="B27" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="C27" s="10" t="n">
+      <c r="C27" s="14" t="n">
         <v>167</v>
       </c>
-      <c r="D27" s="10" t="n">
+      <c r="D27" s="14" t="n">
         <v>120</v>
       </c>
-      <c r="E27" s="10" t="n">
+      <c r="E27" s="14" t="n">
         <v>20</v>
       </c>
       <c r="F27" s="0" t="n">
@@ -3592,16 +3793,16 @@
       <c r="A28" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="10" t="n">
+      <c r="B28" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="C28" s="10" t="n">
+      <c r="C28" s="14" t="n">
         <v>167</v>
       </c>
-      <c r="D28" s="10" t="n">
+      <c r="D28" s="14" t="n">
         <v>110</v>
       </c>
-      <c r="E28" s="10" t="n">
+      <c r="E28" s="14" t="n">
         <v>30</v>
       </c>
       <c r="F28" s="0" t="n">
@@ -3613,16 +3814,16 @@
       <c r="A29" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="10" t="n">
+      <c r="B29" s="14" t="n">
         <v>33</v>
       </c>
-      <c r="C29" s="10" t="n">
+      <c r="C29" s="14" t="n">
         <v>167</v>
       </c>
-      <c r="D29" s="10" t="n">
+      <c r="D29" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="E29" s="10" t="n">
+      <c r="E29" s="14" t="n">
         <v>40</v>
       </c>
       <c r="F29" s="0" t="n">
@@ -3852,7 +4053,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="78.65"/>
@@ -3861,61 +4062,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>150</v>
+        <v>131</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3923,7 +4124,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3931,7 +4132,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3939,7 +4140,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3947,7 +4148,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3955,7 +4156,7 @@
         <v>29</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3963,23 +4164,23 @@
         <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3987,7 +4188,7 @@
         <v>45</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3995,7 +4196,7 @@
         <v>54</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4003,7 +4204,7 @@
         <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4011,7 +4212,7 @@
         <v>54</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4019,7 +4220,7 @@
         <v>53</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4027,7 +4228,7 @@
         <v>53</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4035,7 +4236,7 @@
         <v>53</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -4060,7 +4261,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>
@@ -4070,12 +4271,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -4083,15 +4284,15 @@
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>150</v>
@@ -4108,7 +4309,7 @@
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>100</v>
@@ -4125,7 +4326,7 @@
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>70</v>
@@ -4142,13 +4343,13 @@
     </row>
     <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>365</v>
@@ -4177,7 +4378,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4185,13 +4386,13 @@
         <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4241,35 +4442,35 @@
         <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>50</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>300</v>
@@ -4288,13 +4489,13 @@
         <v>54</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4302,13 +4503,13 @@
         <v>54</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4316,13 +4517,13 @@
         <v>54</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4330,13 +4531,13 @@
         <v>54</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>